<commit_message>
normal version for euler method
</commit_message>
<xml_diff>
--- a/data/_Результаты расчета_.xlsx
+++ b/data/_Результаты расчета_.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet sheetId="1" name="Эйлер при α равен 0 с шагом 0.1" r:id="rId1"/>
+    <sheet sheetId="1" name="Эйлер при α изм. с шагом 0.001" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -74,21 +74,21 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" width="5.5"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" width="24.200000000000003"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="7.700000000000001"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="22.0"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="23.1"/>
     <col min="5" max="5" bestFit="1" customWidth="1" width="23.1"/>
     <col min="6" max="6" bestFit="1" customWidth="1" width="24.200000000000003"/>
     <col min="7" max="7" bestFit="1" customWidth="1" width="24.200000000000003"/>
     <col min="8" max="8" bestFit="1" customWidth="1" width="23.1"/>
-    <col min="9" max="9" bestFit="1" customWidth="1" width="11.0"/>
+    <col min="9" max="9" bestFit="1" customWidth="1" width="28.6"/>
     <col min="10" max="10" bestFit="1" customWidth="1" width="25.3"/>
     <col min="11" max="11" bestFit="1" customWidth="1" width="24.200000000000003"/>
-    <col min="12" max="12" bestFit="1" customWidth="1" width="8.8"/>
+    <col min="12" max="12" bestFit="1" customWidth="1" width="24.200000000000003"/>
     <col min="13" max="13" bestFit="1" customWidth="1" width="23.1"/>
     <col min="14" max="14" bestFit="1" customWidth="1" width="26.400000000000002"/>
     <col min="15" max="15" bestFit="1" customWidth="1" width="24.200000000000003"/>
-    <col min="16" max="16" bestFit="1" customWidth="1" width="26.400000000000002"/>
+    <col min="16" max="16" bestFit="1" customWidth="1" width="27.500000000000004"/>
     <col min="17" max="17" bestFit="1" customWidth="1" width="25.3"/>
     <col min="18" max="18" bestFit="1" customWidth="1" width="23.1"/>
     <col min="19" max="19" bestFit="1" customWidth="1" width="23.1"/>
@@ -279,58 +279,58 @@
         <v>1152.1</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>168105.94939321256</v>
+        <v>168106.62003807584</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>65.83967633292818</v>
+        <v>65.89060420847676</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0.1963867866964461</v>
+        <v>0.19653965962428196</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>160.5835741396591</v>
+        <v>160.8253751754324</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00019627093457359708</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0.012241002645421675</v>
+        <v>0.012292962998523938</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>0.0</v>
+        <v>1.5071342867810773</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>139.44805234213538</v>
+        <v>139.41693217424083</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>-0.11374423067756706</v>
+        <v>-0.08844778863169143</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>-33.72255056932841</v>
+        <v>-34.08982698706482</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>-0.11374423067756706</v>
+        <v>-0.0001465811122509406</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>0.012241002645421675</v>
+        <v>0.012489233933097534</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>1303.4115069507507</v>
+        <v>1303.8342526120387</v>
       </c>
       <c r="S3" s="0" t="n">
-        <v>42.48341900522959</v>
+        <v>42.665954266229015</v>
       </c>
       <c r="T3" s="0" t="n">
-        <v>3.924489817158415</v>
+        <v>4.466743728228738</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>50.29932493832139</v>
+        <v>50.211433653204814</v>
       </c>
     </row>
     <row r="4">
@@ -344,58 +344,58 @@
         <v>1144.2</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>168112.68769581604</v>
+        <v>168114.0622533221</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>79.78448156714171</v>
+        <v>79.88127365365904</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.23799313875400405</v>
+        <v>0.23828426426311808</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>235.7111753300789</v>
+        <v>236.26318542943602</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00032306488919736225</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0.012042481512374525</v>
+        <v>0.012165517849014559</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>0.0</v>
+        <v>3.64440977420921</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>140.4803543394708</v>
+        <v>140.40276406022673</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>-0.09475943951248345</v>
+        <v>-0.060007409552660804</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>-49.49934681931657</v>
+        <v>-50.3805949927655</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>-0.09475943951248345</v>
+        <v>-0.0006811421424435144</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>0.012042481512374525</v>
+        <v>0.01248858273821192</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>1307.6598488512736</v>
+        <v>1308.526695040077</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>50.78476549780328</v>
+        <v>51.279419093845604</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>8.954422310990555</v>
+        <v>10.033652047425177</v>
       </c>
       <c r="U4" s="0" t="n">
-        <v>61.53430825377583</v>
+        <v>61.24899230133099</v>
       </c>
     </row>
     <row r="5">
@@ -403,64 +403,64 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.30000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1136.3</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>168120.7389512286</v>
+        <v>168122.87096138892</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>93.83251700108879</v>
+        <v>93.9696929915025</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.27991424368663453</v>
+        <v>0.28032783829757885</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>325.86067616681436</v>
+        <v>326.77066525913017</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0004101349494101655</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.011877095090690803</v>
+        <v>0.012076429698151654</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0.0</v>
+        <v>6.398986996848839</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>141.50008831800997</v>
+        <v>141.3737033771288</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>-0.08119899848976289</v>
+        <v>-0.043269559445906706</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>-68.43074199503101</v>
+        <v>-69.96562697375559</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>-0.08119899848976289</v>
+        <v>-0.0017407432919961286</v>
       </c>
       <c r="Q5" s="0" t="n">
-        <v>0.011877095090690803</v>
+        <v>0.012486564647561817</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>1312.738325401054</v>
+        <v>1314.083558357746</v>
       </c>
       <c r="S5" s="0" t="n">
-        <v>59.038246811563496</v>
+        <v>59.95485452421697</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>15.107853136368139</v>
+        <v>16.70785890146968</v>
       </c>
       <c r="U5" s="0" t="n">
-        <v>72.93165746215102</v>
+        <v>72.35826573306751</v>
       </c>
     </row>
     <row r="6">
@@ -474,58 +474,58 @@
         <v>1128.4</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>168130.0935900059</v>
+        <v>168133.0536328496</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>107.98252583288979</v>
+        <v>108.15482143877472</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.3221476036894878</v>
+        <v>0.32266862544663194</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>431.29916009998067</v>
+        <v>432.5966408948018</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00047145581884123756</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.011735376103393976</v>
+        <v>0.012010692276678205</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0.0</v>
+        <v>9.737904912400746</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>142.51084953774398</v>
+        <v>142.33776048756386</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>-0.071020021772676</v>
+        <v>-0.03271816508275411</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>-90.57282362099593</v>
+        <v>-92.89025461951253</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>-0.071020021772676</v>
+        <v>-0.0034574928754325905</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>0.011735376103393976</v>
+        <v>0.012482148095519443</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>1318.6421500822103</v>
+        <v>1320.510989090177</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>67.25752163233749</v>
+        <v>68.69113223119206</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>22.40101888258324</v>
+        <v>24.496586698781712</v>
       </c>
       <c r="U6" s="0" t="n">
-        <v>84.4787054181488</v>
+        <v>83.54037199612013</v>
       </c>
     </row>
     <row r="7">
@@ -539,58 +539,58 @@
         <v>1120.5</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>168140.74390185592</v>
+        <v>168144.61712607933</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>122.23361078666419</v>
+        <v>122.43618594380513</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.3646918077647008</v>
+        <v>0.3653065927640621</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>552.2859730267312</v>
+        <v>553.983953622601</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0005140974829107041</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.011611422781916849</v>
+        <v>0.01195998155758147</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>0.0</v>
+        <v>13.598282186816903</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>143.51481870761785</v>
+        <v>143.29886952668278</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>-0.06309290170768653</v>
+        <v>-0.025793230768744367</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>-115.98005433561354</v>
+        <v>-119.19226951997777</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>-0.06309290170768653</v>
+        <v>-0.005953004950027824</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>0.011611422781916849</v>
+        <v>0.012474079040492173</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>1325.367902245444</v>
+        <v>1327.8149860089356</v>
       </c>
       <c r="S7" s="0" t="n">
-        <v>75.4528262502009</v>
+        <v>77.48638527542693</v>
       </c>
       <c r="T7" s="0" t="n">
-        <v>30.848889424398124</v>
+        <v>33.40719873085694</v>
       </c>
       <c r="U7" s="0" t="n">
-        <v>96.16614069828685</v>
+        <v>94.79704491920687</v>
       </c>
     </row>
     <row r="8">
@@ -604,58 +604,58 @@
         <v>1112.6</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>168152.68349308486</v>
+        <v>168157.5675491743</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>136.58509265742597</v>
+        <v>136.8136120297295</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0.4075461115492172</v>
+        <v>0.40824262765949665</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>689.0728825482964</v>
+        <v>691.1693631187948</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00054168514947129</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0.011501304894973221</v>
+        <v>0.011919220597803605</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>0.0</v>
+        <v>17.876100805582034</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>144.51338819028337</v>
+        <v>144.25927723976054</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>-0.05674175836987858</v>
+        <v>-0.021182309000094567</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>-144.70530533514224</v>
+        <v>-148.89954742411913</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>-0.05674175836987858</v>
+        <v>-0.009330493178224781</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>0.011501304894973221</v>
+        <v>0.012460905747274894</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>1332.913184870464</v>
+        <v>1336.0013169713848</v>
       </c>
       <c r="S8" s="0" t="n">
-        <v>83.63211213014976</v>
+        <v>86.33782451735766</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>40.46550349422681</v>
+        <v>43.44726865384672</v>
       </c>
       <c r="U8" s="0" t="n">
-        <v>107.98683881329102</v>
+        <v>106.13078956754869</v>
       </c>
     </row>
     <row r="9">
@@ -669,58 +669,58 @@
         <v>1104.7</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>168165.90692396968</v>
+        <v>168171.91009586924</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>151.0364314764543</v>
+        <v>151.28710604737114</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.45071020356223335</v>
+        <v>0.45147818617395163</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>841.904064154388</v>
+        <v>844.3834863192506</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0005559638929872189</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>0.01140227184428068</v>
+        <v>0.011885055677803817</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>0.0</v>
+        <v>22.41443029024225</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>145.50747570663322</v>
+        <v>145.22043387443904</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>-0.05153717018793854</v>
+        <v>-0.01816052426112437</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>-176.7998534724215</v>
+        <v>-182.02756248799344</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>-0.05153717018793854</v>
+        <v>-0.013664300561570766</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <v>0.01140227184428068</v>
+        <v>0.012441019570791035</v>
       </c>
       <c r="R9" s="0" t="n">
-        <v>1341.2763960834789</v>
+        <v>1345.0754186024517</v>
       </c>
       <c r="S9" s="0" t="n">
-        <v>91.8017272361797</v>
+        <v>95.24157920075268</v>
       </c>
       <c r="T9" s="0" t="n">
-        <v>51.26418737555591</v>
+        <v>54.62466429785385</v>
       </c>
       <c r="U9" s="0" t="n">
-        <v>119.93517628117175</v>
+        <v>117.5450128569276</v>
       </c>
     </row>
     <row r="10">
@@ -728,64 +728,64 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1096.8</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>168180.4094538048</v>
+        <v>168187.6488599652</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>165.58717904711764</v>
+        <v>165.85679544140004</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.49418406477731874</v>
+        <v>0.4950151139021945</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>1011.015982847052</v>
+        <v>1013.850732391546</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0005576045388819591</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0.01131232251358666</v>
+        <v>0.011855111666463044</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0.0</v>
+        <v>26.992412725007966</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>146.49769600038724</v>
+        <v>146.1833397310556</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>-0.04719308896159139</v>
+        <v>-0.016302610211186976</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>-212.3133563978809</v>
+        <v>-218.5770604744763</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>-0.04719308896159139</v>
+        <v>-0.018986932960047963</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>0.01131232251358666</v>
+        <v>0.012412716205345004</v>
       </c>
       <c r="R10" s="0" t="n">
-        <v>1350.4565688070968</v>
+        <v>1355.042281399539</v>
       </c>
       <c r="S10" s="0" t="n">
-        <v>99.96684943569828</v>
+        <v>104.19256672837069</v>
       </c>
       <c r="T10" s="0" t="n">
-        <v>63.25770500367309</v>
+        <v>66.94764307469592</v>
       </c>
       <c r="U10" s="0" t="n">
-        <v>132.00660164810935</v>
+        <v>129.04412281326273</v>
       </c>
     </row>
     <row r="11">
@@ -793,64 +793,64 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1088.9</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>168196.18685439136</v>
+        <v>168204.78663426402</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>180.23694864715637</v>
+        <v>180.52289075830456</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.5379678792227449</v>
+        <v>0.5388555313321042</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>1196.6372078108627</v>
+        <v>1199.7891777626353</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0005466790053450764</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.011229955034930024</v>
+        <v>0.011827602419790846</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>0.0</v>
+        <v>31.316896872686055</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>147.48446140334278</v>
+        <v>147.14866111150172</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>-0.04351153857844028</v>
+        <v>-0.015344472893727526</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>-251.29381364028117</v>
+        <v>-258.5322756734175</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>-0.04351153857844028</v>
+        <v>-0.02527405679299576</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <v>0.011229955034930024</v>
+        <v>0.012374281425135922</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>1360.4532537506666</v>
+        <v>1365.9063237604262</v>
       </c>
       <c r="S11" s="0" t="n">
-        <v>108.13177555524223</v>
+        <v>113.18440435178925</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>76.45836516848402</v>
+        <v>80.42495522880935</v>
       </c>
       <c r="U11" s="0" t="n">
-        <v>144.19735355722864</v>
+        <v>140.6335831132288</v>
       </c>
     </row>
     <row r="12">
@@ -858,64 +858,64 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.9999999999999999</v>
+        <v>1.0</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1081.0</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>168213.23526914485</v>
+        <v>168223.32467263535</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>194.98539478749063</v>
+        <v>195.28434083158984</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.5820619744483205</v>
+        <v>0.5829978172118397</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.30910345016108876</v>
+        <v>0.30946237604230875</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>1441.4402463636986</v>
+        <v>1446.6246488553836</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0005229558473667991</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0.011154013073849793</v>
+        <v>0.01180111780894795</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>0.0</v>
+        <v>35.01673660662841</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>148.42877294587666</v>
+        <v>148.07584440361418</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>-0.04035109708436596</v>
+        <v>-0.015112408981870096</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>-302.7024517363767</v>
+        <v>-311.1446909470225</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>-0.04035109708436596</v>
+        <v>-0.03250384819654768</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <v>0.011154013073849793</v>
+        <v>0.01232407365631475</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>1371.2664313061907</v>
+        <v>1377.6712410505493</v>
       </c>
       <c r="S12" s="0" t="n">
-        <v>116.30012167446672</v>
+        <v>122.2085551113835</v>
       </c>
       <c r="T12" s="0" t="n">
-        <v>90.87810052420689</v>
+        <v>95.0659261867646</v>
       </c>
       <c r="U12" s="0" t="n">
-        <v>156.5042679256314</v>
+        <v>152.3188853413013</v>
       </c>
     </row>
     <row r="13">
@@ -923,64 +923,64 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1.0999999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1073.1</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>168231.55110379966</v>
+        <v>168243.26210793102</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>209.82827208207829</v>
+        <v>210.13452172011782</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.6264550558236511</v>
+        <v>0.627423729621186</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.33256029702528855</v>
+        <v>0.3332186034115341</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>1793.8528452726348</v>
+        <v>1801.3257055012673</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0004858105386265127</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0.011083587123758386</v>
+        <v>0.011774493362369989</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>0.0</v>
+        <v>37.617729524559394</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>149.28500428112494</v>
+        <v>148.92048501242857</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>-0.0376087246948573</v>
+        <v>-0.015497360211948932</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>-376.7090975072533</v>
+        <v>-386.1781213554236</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>-0.0376087246948573</v>
+        <v>-0.04085275263377205</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>0.011083587123758386</v>
+        <v>0.0122603039009965</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>1382.8964434736374</v>
+        <v>1390.3396338732905</v>
       </c>
       <c r="S13" s="0" t="n">
-        <v>124.47263675682531</v>
+        <v>131.25158906773777</v>
       </c>
       <c r="T13" s="0" t="n">
-        <v>106.52852731677002</v>
+        <v>110.88026618798101</v>
       </c>
       <c r="U13" s="0" t="n">
-        <v>168.92148017275392</v>
+        <v>164.10221688245522</v>
       </c>
     </row>
     <row r="14">
@@ -994,58 +994,58 @@
         <v>1065.2</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>168251.13057348676</v>
+        <v>168264.59529841036</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>224.75677251019079</v>
+        <v>225.06390526934837</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.6711222179918708</v>
+        <v>0.6721063558379781</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.3694221918345353</v>
+        <v>0.3703841158507817</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>2283.5022327802917</v>
+        <v>2293.7611418756323</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0004342069539939085</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.01101794751641825</v>
+        <v>0.01174671175545336</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0.0</v>
+        <v>38.517248313308016</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>150.0237393567984</v>
+        <v>149.65260723332065</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>-0.0352076418091394</v>
+        <v>-0.016435771586507372</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>-479.53546888386126</v>
+        <v>-489.7784619396774</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>-0.0352076418091394</v>
+        <v>-0.05041188895113269</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>0.01101794751641825</v>
+        <v>0.012180918709447269</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>1395.34370714932</v>
+        <v>1403.9125867654939</v>
       </c>
       <c r="S14" s="0" t="n">
-        <v>132.64696936680974</v>
+        <v>140.29664425187443</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>123.42067533404541</v>
+        <v>127.87784346675505</v>
       </c>
       <c r="U14" s="0" t="n">
-        <v>181.4397649552002</v>
+        <v>175.98469554695149</v>
       </c>
     </row>
     <row r="15">
@@ -1059,58 +1059,58 @@
         <v>1057.3</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>168271.96921616452</v>
+        <v>168287.31726897</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>239.7591464458706</v>
+        <v>240.05931011231405</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.716029772108374</v>
+        <v>0.7170078591381525</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.4198910752063798</v>
+        <v>0.4211398885359654</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>2949.6401771081855</v>
+        <v>2962.9510283745817</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0003670278395011614</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0.01095649858927502</v>
+        <v>0.011716845678943013</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0.0</v>
+        <v>36.98790589429482</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>150.60551455971617</v>
+        <v>150.23222145614815</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>-0.033089214806015205</v>
+        <v>-0.017884225600787562</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>-619.424437192719</v>
+        <v>-629.987176196464</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>-0.033089214806015205</v>
+        <v>-0.061049767029402235</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>0.01095649858927502</v>
+        <v>0.012083873518444171</v>
       </c>
       <c r="R15" s="0" t="n">
-        <v>1408.608404086001</v>
+        <v>1418.3893021487486</v>
       </c>
       <c r="S15" s="0" t="n">
-        <v>140.81874940803363</v>
+        <v>149.32280520812492</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>141.56465182956543</v>
+        <v>146.06856623140928</v>
       </c>
       <c r="U15" s="0" t="n">
-        <v>194.04774700987863</v>
+        <v>187.96588045806757</v>
       </c>
     </row>
     <row r="16">
@@ -1118,64 +1118,64 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1.4000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1049.4</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>168294.06157968193</v>
+        <v>168311.41707163723</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>254.81969790184223</v>
+        <v>255.103260005347</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.7611322327870182</v>
+        <v>0.7620775407076884</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0.4841112447625169</v>
+        <v>0.4856023407726262</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>3836.0740029407743</v>
+        <v>3852.22488539682</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00028364968569279467</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0.010898747014748559</v>
+        <v>0.011684044593205852</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>0.0</v>
+        <v>32.23115054689617</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>150.98528568625207</v>
+        <v>150.61338199717233</v>
       </c>
       <c r="N16" s="0" t="n">
-        <v>-0.03120800115446182</v>
+        <v>-0.019793354575481027</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>-805.5755406175625</v>
+        <v>-815.7357675481803</v>
       </c>
       <c r="P16" s="0" t="n">
-        <v>-0.03120800115446182</v>
+        <v>-0.07219801179978172</v>
       </c>
       <c r="Q16" s="0" t="n">
-        <v>0.010898747014748559</v>
+        <v>0.011967694278898648</v>
       </c>
       <c r="R16" s="0" t="n">
-        <v>1422.6902790268043</v>
+        <v>1433.766677258994</v>
       </c>
       <c r="S16" s="0" t="n">
-        <v>148.98108666535094</v>
+        <v>158.30483866590424</v>
       </c>
       <c r="T16" s="0" t="n">
-        <v>160.9694265305533</v>
+        <v>165.46219599087405</v>
       </c>
       <c r="U16" s="0" t="n">
-        <v>206.73101909195276</v>
+        <v>200.04312365167092</v>
       </c>
     </row>
     <row r="17">
@@ -1183,64 +1183,64 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1.5000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1041.5</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>168317.40083369327</v>
+        <v>168336.87916101245</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>269.91822647046746</v>
+        <v>270.1736319752054</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.8063706340176006</v>
+        <v>0.8072507621711561</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0.5592374193255208</v>
+        <v>0.5605136051481764</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>4964.721509289102</v>
+        <v>4979.3195013246195</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00018489821596606742</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0.010844278777437405</v>
+        <v>0.011647571411138497</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>0.24681468299119974</v>
+        <v>0.24637461891442197</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>0.0</v>
+        <v>23.186497719327768</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>151.1376183715887</v>
+        <v>150.77259859422003</v>
       </c>
       <c r="N17" s="0" t="n">
-        <v>-0.02952828523195355</v>
+        <v>-0.02207731870722684</v>
       </c>
       <c r="O17" s="0" t="n">
-        <v>-1042.5915169507114</v>
+        <v>-1050.5262597992287</v>
       </c>
       <c r="P17" s="0" t="n">
-        <v>-0.02952828523195355</v>
+        <v>-0.0825761185969524</v>
       </c>
       <c r="Q17" s="0" t="n">
-        <v>0.010844278777437405</v>
+        <v>0.011832469627104566</v>
       </c>
       <c r="R17" s="0" t="n">
-        <v>1437.5883876933394</v>
+        <v>1450.0388839526183</v>
       </c>
       <c r="S17" s="0" t="n">
-        <v>157.12432502606177</v>
+        <v>167.21368432643027</v>
       </c>
       <c r="T17" s="0" t="n">
-        <v>181.6425284397486</v>
+        <v>186.0680797888292</v>
       </c>
       <c r="U17" s="0" t="n">
-        <v>219.47162792959605</v>
+        <v>212.21068584935745</v>
       </c>
     </row>
     <row r="18">
@@ -1248,64 +1248,64 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1.6000000000000003</v>
+        <v>1.6</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1033.6</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>168341.97834776682</v>
+        <v>168363.68338141887</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>285.0319883076263</v>
+        <v>285.2561349370442</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0.8516783674102439</v>
+        <v>0.8524862110468538</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0.6249336327448537</v>
+        <v>0.626105006017938</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>6177.012434909664</v>
+        <v>6189.7867422810305</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>0.0</v>
+        <v>7.454048562202094e-05</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0.010792742197460844</v>
+        <v>0.011606897795673756</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>0.22416081629487805</v>
+        <v>0.2237568944765731</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>0.0</v>
+        <v>9.447562775086723</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>151.21088823425262</v>
+        <v>150.85181114364943</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>-0.02802140617618017</v>
+        <v>-0.02456906760873406</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>-1297.1726113310294</v>
+        <v>-1301.8392040617844</v>
       </c>
       <c r="P18" s="0" t="n">
-        <v>-0.02802140617618017</v>
+        <v>-0.08979525708791428</v>
       </c>
       <c r="Q18" s="0" t="n">
-        <v>0.010792742197460844</v>
+        <v>0.011681438281295775</v>
       </c>
       <c r="R18" s="0" t="n">
-        <v>1453.3008201959456</v>
+        <v>1467.1973330310077</v>
       </c>
       <c r="S18" s="0" t="n">
-        <v>165.23724964703035</v>
+        <v>176.02579713701024</v>
       </c>
       <c r="T18" s="0" t="n">
-        <v>203.5896912327082</v>
+        <v>207.89513461188005</v>
       </c>
       <c r="U18" s="0" t="n">
-        <v>232.2496193488458</v>
+        <v>224.46821882284647</v>
       </c>
     </row>
     <row r="19">
@@ -1313,64 +1313,64 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>1.7000000000000004</v>
+        <v>1.7</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1025.7</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>168367.78346349366</v>
+        <v>168391.8062170177</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>300.1530771310516</v>
+        <v>300.3384828918244</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.8970331096692391</v>
+        <v>0.8977485022880672</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0.6906980090203966</v>
+        <v>0.6917353283176976</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>7558.212365757917</v>
+        <v>7567.335809260787</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>0.0</v>
+        <v>-3.9246944842947456e-05</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0.010743835617579542</v>
+        <v>0.011561897738884414</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>0.20148344516538047</v>
+        <v>0.2011257488559664</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>0.0</v>
+        <v>-4.947652756088901</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>151.12028820004994</v>
+        <v>150.76567638596336</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>-0.026662552574470883</v>
+        <v>-0.026978957547575642</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>-1587.2245968091624</v>
+        <v>-1588.1015128659865</v>
       </c>
       <c r="P19" s="0" t="n">
-        <v>-0.026662552574470883</v>
+        <v>-0.09090620162253321</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <v>0.010743835617579542</v>
+        <v>0.011522650794041465</v>
       </c>
       <c r="R19" s="0" t="n">
-        <v>1469.8245451606485</v>
+        <v>1485.2314452463575</v>
       </c>
       <c r="S19" s="0" t="n">
-        <v>173.31716458291535</v>
+        <v>184.7228443521715</v>
       </c>
       <c r="T19" s="0" t="n">
-        <v>226.81465316759278</v>
+        <v>230.95235828615816</v>
       </c>
       <c r="U19" s="0" t="n">
-        <v>245.05719775631493</v>
+        <v>236.8135871950892</v>
       </c>
     </row>
     <row r="20">
@@ -1378,64 +1378,64 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1.8000000000000005</v>
+        <v>1.8</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1017.8</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>168394.80484078833</v>
+        <v>168421.22133070498</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>315.26510595105657</v>
+        <v>315.40354806529064</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0.9423871647305778</v>
+        <v>0.9429877081747593</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0.7564613888593378</v>
+        <v>0.757332176853401</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>9116.679010563192</v>
+        <v>9119.806779600885</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00014373544029547806</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0.010697300684638481</v>
+        <v>0.011513012801548435</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>0.24238716473057786</v>
+        <v>0.24298770817475934</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>0.0</v>
+        <v>-24.09739124178378</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>150.85391800748727</v>
+        <v>150.50278378752535</v>
       </c>
       <c r="N20" s="0" t="n">
-        <v>-0.02543213934704106</v>
+        <v>-0.028953568675741323</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>-1914.5025922182701</v>
+        <v>-1910.098971555411</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>-0.02543213934704106</v>
+        <v>-0.08307700806118208</v>
       </c>
       <c r="Q20" s="0" t="n">
-        <v>0.010697300684638481</v>
+        <v>0.011369277361252955</v>
       </c>
       <c r="R20" s="0" t="n">
-        <v>1487.15626161894</v>
+        <v>1504.1289701898415</v>
       </c>
       <c r="S20" s="0" t="n">
-        <v>181.35636421500706</v>
+        <v>193.29127344123367</v>
       </c>
       <c r="T20" s="0" t="n">
-        <v>251.32037294322427</v>
+        <v>255.24800053500215</v>
       </c>
       <c r="U20" s="0" t="n">
-        <v>257.8797320245324</v>
+        <v>249.23459178781812</v>
       </c>
     </row>
     <row r="21">
@@ -1443,64 +1443,64 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1.9000000000000006</v>
+        <v>1.9</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1009.9</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>168423.0296883476</v>
+        <v>168451.90086921238</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>330.3504977518053</v>
+        <v>330.43324295289204</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>0.9876892261889803</v>
+        <v>0.9881509520701702</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0.8221493779740213</v>
+        <v>0.8228188805017468</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>10859.668706587483</v>
+        <v>10853.898004763661</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00022261955462132265</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0.010652913227895293</v>
+        <v>0.011461352862401953</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>0.2876892261889803</v>
+        <v>0.2881509520701703</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>0.0</v>
+        <v>-48.482777116175185</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>150.40057623466268</v>
+        <v>150.05545407961878</v>
       </c>
       <c r="N21" s="0" t="n">
-        <v>-0.024313977620416774</v>
+        <v>-0.030078236163631627</v>
       </c>
       <c r="O21" s="0" t="n">
-        <v>-2280.530428383371</v>
+        <v>-2269.137197805972</v>
       </c>
       <c r="P21" s="0" t="n">
-        <v>-0.024313977620416774</v>
+        <v>-0.06448582878520487</v>
       </c>
       <c r="Q21" s="0" t="n">
-        <v>0.010652913227895293</v>
+        <v>0.011238733307780628</v>
       </c>
       <c r="R21" s="0" t="n">
-        <v>1505.2918980404409</v>
+        <v>1523.87680022549</v>
       </c>
       <c r="S21" s="0" t="n">
-        <v>189.34640204408777</v>
+        <v>201.72829329372402</v>
       </c>
       <c r="T21" s="0" t="n">
-        <v>277.1083461456775</v>
+        <v>280.7886364309503</v>
       </c>
       <c r="U21" s="0" t="n">
-        <v>270.7016649336021</v>
+        <v>261.7094261450402</v>
       </c>
     </row>
     <row r="22">
@@ -1508,64 +1508,64 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>2.0000000000000004</v>
+        <v>2.0</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1002.0</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>168452.44366596133</v>
+        <v>168483.81779119174</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>345.39055537527156</v>
+        <v>345.42369921082104</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>1.032884574910142</v>
+        <v>1.0332278185170276</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>0.8575900902570202</v>
+        <v>0.8577337743041666</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>12359.46289679331</v>
+        <v>12339.06285422902</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.0002591123752311062</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>0.010610477331522044</v>
+        <v>0.011408766934796642</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>0.30548076248502365</v>
+        <v>0.3055379697528379</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>0.0</v>
+        <v>-65.25377506056091</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>150.1827983060868</v>
+        <v>149.85396031531099</v>
       </c>
       <c r="N22" s="0" t="n">
-        <v>-0.02329456577581419</v>
+        <v>-0.029941873631207944</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>-2595.487208326595</v>
+        <v>-2577.4999066253763</v>
       </c>
       <c r="P22" s="0" t="n">
-        <v>-0.02329456577581419</v>
+        <v>-0.036010666325228625</v>
       </c>
       <c r="Q22" s="0" t="n">
-        <v>0.010610477331522044</v>
+        <v>0.011149654559565536</v>
       </c>
       <c r="R22" s="0" t="n">
-        <v>1524.2265382448497</v>
+        <v>1544.4624530317978</v>
       </c>
       <c r="S22" s="0" t="n">
-        <v>197.27815148539284</v>
+        <v>210.05466659004318</v>
       </c>
       <c r="T22" s="0" t="n">
-        <v>304.1785126390377</v>
+        <v>307.5783618720802</v>
       </c>
       <c r="U22" s="0" t="n">
-        <v>283.5065549311778</v>
+        <v>274.2162814645286</v>
       </c>
     </row>
     <row r="23">
@@ -1573,64 +1573,64 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2.1000000000000005</v>
+        <v>2.1</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>994.0999999999999</v>
+        <v>994.1</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>168483.03079900428</v>
+        <v>168516.95151374413</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>360.4088352058802</v>
+        <v>360.40986919660816</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>1.0780448054138887</v>
+        <v>1.078324055187903</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0.8694106527367067</v>
+        <v>0.8694393341983657</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>13616.426834165035</v>
+        <v>13587.299841800881</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00024248477467904344</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>0.01056982064446101</v>
+        <v>0.011357671826192628</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>0.2829327918791671</v>
+        <v>0.28251391721814567</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>0.0</v>
+        <v>-61.33958446225678</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>150.20591216315654</v>
+        <v>149.89504839967285</v>
       </c>
       <c r="N23" s="0" t="n">
-        <v>-0.02235986500881439</v>
+        <v>-0.02834391892405856</v>
       </c>
       <c r="O23" s="0" t="n">
-        <v>-2859.449635174657</v>
+        <v>-2840.451654041111</v>
       </c>
       <c r="P23" s="0" t="n">
-        <v>-0.02235986500881439</v>
+        <v>-0.002977618059728073</v>
       </c>
       <c r="Q23" s="0" t="n">
-        <v>0.01056982064446101</v>
+        <v>0.011115187051513585</v>
       </c>
       <c r="R23" s="0" t="n">
-        <v>1543.954353393389</v>
+        <v>1565.8777194202876</v>
       </c>
       <c r="S23" s="0" t="n">
-        <v>205.16651412357862</v>
+        <v>218.32932176447494</v>
       </c>
       <c r="T23" s="0" t="n">
-        <v>332.52916813215546</v>
+        <v>335.62041759004745</v>
       </c>
       <c r="U23" s="0" t="n">
-        <v>296.31272327869885</v>
+        <v>286.7535197206489</v>
       </c>
     </row>
     <row r="24">
@@ -1638,64 +1638,64 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>2.2000000000000006</v>
+        <v>2.2</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>986.1999999999999</v>
+        <v>986.2</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>168514.77721503822</v>
+        <v>168551.29018922543</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>375.4294264221959</v>
+        <v>375.4084889236077</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>1.1232431775427114</v>
+        <v>1.1234910584879778</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.8669469825648779</v>
+        <v>0.8668940426745024</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>14703.152159192932</v>
+        <v>14666.066017702266</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.0001736200094163857</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>0.010530795317990482</v>
+        <v>0.011310544372381916</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>0.0</v>
+        <v>-42.07363486731429</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>150.4021685401393</v>
+        <v>150.11346787576275</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>-0.021498307037238498</v>
+        <v>-0.02545862054504082</v>
       </c>
       <c r="O24" s="0" t="n">
-        <v>-3087.6619534305155</v>
+        <v>-3071.03840039534</v>
       </c>
       <c r="P24" s="0" t="n">
-        <v>-0.021498307037238498</v>
+        <v>0.026953071536084956</v>
       </c>
       <c r="Q24" s="0" t="n">
-        <v>0.010530795317990482</v>
+        <v>0.011136924362965532</v>
       </c>
       <c r="R24" s="0" t="n">
-        <v>1564.4710048057468</v>
+        <v>1588.1201755987597</v>
       </c>
       <c r="S24" s="0" t="n">
-        <v>213.0264456380974</v>
+        <v>226.60785155616145</v>
       </c>
       <c r="T24" s="0" t="n">
-        <v>362.16044046002537</v>
+        <v>364.9168155113905</v>
       </c>
       <c r="U24" s="0" t="n">
-        <v>309.1391073327633</v>
+        <v>299.2998749899625</v>
       </c>
     </row>
     <row r="25">
@@ -1703,64 +1703,64 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>2.3000000000000007</v>
+        <v>2.3</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>978.3</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>168547.67113670398</v>
+        <v>168586.8301714391</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>390.4696432762098</v>
+        <v>390.4399419627784</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>1.1685327599316073</v>
+        <v>1.1687912721024953</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0.8501347748599688</v>
+        <v>0.8499975994836975</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>15563.353705406083</v>
+        <v>15519.157294864619</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>0.0</v>
+        <v>-6.704645402630597e-05</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>0.010493273693850034</v>
+        <v>0.011269210356126826</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>0.0</v>
+        <v>-17.534318481632152</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>150.83335659212293</v>
+        <v>150.56358098014192</v>
       </c>
       <c r="N25" s="0" t="n">
-        <v>-0.020700664537021008</v>
+        <v>-0.02179190989005407</v>
       </c>
       <c r="O25" s="0" t="n">
-        <v>-3268.3042781352774</v>
+        <v>-3255.3408250404277</v>
       </c>
       <c r="P25" s="0" t="n">
-        <v>-0.020700664537021008</v>
+        <v>0.04547895903647871</v>
       </c>
       <c r="Q25" s="0" t="n">
-        <v>0.010493273693850034</v>
+        <v>0.01120216390210052</v>
       </c>
       <c r="R25" s="0" t="n">
-        <v>1585.7736493695566</v>
+        <v>1611.1928947548702</v>
       </c>
       <c r="S25" s="0" t="n">
-        <v>220.8688438537097</v>
+        <v>234.94342561756747</v>
       </c>
       <c r="T25" s="0" t="n">
-        <v>393.0743511933017</v>
+        <v>395.46766475830873</v>
       </c>
       <c r="U25" s="0" t="n">
-        <v>321.99921759994413</v>
+        <v>311.84120163791744</v>
       </c>
     </row>
     <row r="26">
@@ -1768,64 +1768,64 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>2.400000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>970.4</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>168581.7022390404</v>
+        <v>168623.57493809995</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>405.5529789354221</v>
+        <v>405.5287215401484</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>1.2139851850829018</v>
+        <v>1.2142995968082342</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.8246015113686427</v>
+        <v>0.8244846397455847</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>16248.952629771204</v>
+        <v>16200.688905092875</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>0.0</v>
+        <v>5.089471805229354e-05</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>0.01045714421849785</v>
+        <v>0.011234457808314932</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>0.0</v>
+        <v>14.324724142005381</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>151.45176336285527</v>
+        <v>151.18906321793108</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>-0.019958883658343286</v>
+        <v>-0.018047346179833768</v>
       </c>
       <c r="O26" s="0" t="n">
-        <v>-3412.280052251953</v>
+        <v>-3405.152862139325</v>
       </c>
       <c r="P26" s="0" t="n">
-        <v>-0.019958883658343286</v>
+        <v>0.04673269689930805</v>
       </c>
       <c r="Q26" s="0" t="n">
-        <v>0.01045714421849785</v>
+        <v>0.011285352526367226</v>
       </c>
       <c r="R26" s="0" t="n">
-        <v>1607.8605337549275</v>
+        <v>1635.103807110926</v>
       </c>
       <c r="S26" s="0" t="n">
-        <v>228.70792156532173</v>
+        <v>243.377541786203</v>
       </c>
       <c r="T26" s="0" t="n">
-        <v>425.27427295329613</v>
+        <v>427.27236239585034</v>
       </c>
       <c r="U26" s="0" t="n">
-        <v>334.911787395824</v>
+        <v>324.3777368255908</v>
       </c>
     </row>
     <row r="27">
@@ -1833,64 +1833,64 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>2.500000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>962.5</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>168616.86214494825</v>
+        <v>168661.53119329773</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>420.69815527170766</v>
+        <v>420.66942490417085</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>1.2596578997307033</v>
+        <v>1.2600015365698547</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.8096959051079977</v>
+        <v>0.8095995697628022</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>17130.10446826297</v>
+        <v>17076.082964304584</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00014886860760997215</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>0.010422309395011792</v>
+        <v>0.01120574726843286</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>0.0</v>
+        <v>44.976303087318186</v>
       </c>
       <c r="M27" s="0" t="n">
-        <v>151.8774706286427</v>
+        <v>151.6155293424898</v>
       </c>
       <c r="N27" s="0" t="n">
-        <v>-0.019266408957164447</v>
+        <v>-0.014996172021367772</v>
       </c>
       <c r="O27" s="0" t="n">
-        <v>-3597.3219383352234</v>
+        <v>-3595.4224461523</v>
       </c>
       <c r="P27" s="0" t="n">
-        <v>-0.019266408957164447</v>
+        <v>0.029566964856484076</v>
       </c>
       <c r="Q27" s="0" t="n">
-        <v>0.010422309395011792</v>
+        <v>0.011354615876042834</v>
       </c>
       <c r="R27" s="0" t="n">
-        <v>1630.7313259114596</v>
+        <v>1659.8632151582046</v>
       </c>
       <c r="S27" s="0" t="n">
-        <v>236.5550248632556</v>
+        <v>251.910352815453</v>
       </c>
       <c r="T27" s="0" t="n">
-        <v>458.7654516928785</v>
+        <v>460.3302657548388</v>
       </c>
       <c r="U27" s="0" t="n">
-        <v>347.891733246081</v>
+        <v>336.9034567848775</v>
       </c>
     </row>
     <row r="28">
@@ -1898,64 +1898,64 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>2.600000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>954.5999999999999</v>
+        <v>954.6</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>168653.1439646187</v>
+        <v>168700.70240653932</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>435.88590233457194</v>
+        <v>435.848533994141</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>1.3054946545816295</v>
+        <v>1.3058582721045409</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0.7989312603126457</v>
+        <v>0.7988626649311432</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>18102.069278669547</v>
+        <v>18041.393375730364</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00019919979106830255</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>0.010388683167877966</v>
+        <v>0.011181305407491795</v>
       </c>
       <c r="K28" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>0.0</v>
+        <v>64.43910070616023</v>
       </c>
       <c r="M28" s="0" t="n">
-        <v>152.21546009420965</v>
+        <v>151.95460788955776</v>
       </c>
       <c r="N28" s="0" t="n">
-        <v>-0.018619289253354036</v>
+        <v>-0.013246529865917773</v>
       </c>
       <c r="O28" s="0" t="n">
-        <v>-3801.434548520605</v>
+        <v>-3802.2248200516706</v>
       </c>
       <c r="P28" s="0" t="n">
-        <v>-0.018619289253354036</v>
+        <v>-0.0020033727375021273</v>
       </c>
       <c r="Q28" s="0" t="n">
-        <v>0.010388683167877966</v>
+        <v>0.011380505198560096</v>
       </c>
       <c r="R28" s="0" t="n">
-        <v>1654.3868283977852</v>
+        <v>1685.4795979094179</v>
       </c>
       <c r="S28" s="0" t="n">
-        <v>244.4000527142947</v>
+        <v>260.51100567922936</v>
       </c>
       <c r="T28" s="0" t="n">
-        <v>493.5546250174866</v>
+        <v>494.64037981036864</v>
       </c>
       <c r="U28" s="0" t="n">
-        <v>360.9226150953608</v>
+        <v>349.4251858478985</v>
       </c>
     </row>
     <row r="29">
@@ -1963,64 +1963,64 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2.700000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>946.6999999999999</v>
+        <v>946.7</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>168690.53899956346</v>
+        <v>168741.08550742696</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>451.1074483439929</v>
+        <v>451.05672482874303</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>1.3514705869921806</v>
+        <v>1.3518434743388172</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.7923551039268839</v>
+        <v>0.7923190509637563</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>19182.03987322788</v>
+        <v>19113.572996037237</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00018641373728773254</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>0.010356186377692743</v>
+        <v>0.011158569124212642</v>
       </c>
       <c r="K29" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>0.0</v>
+        <v>64.41430651367533</v>
       </c>
       <c r="M29" s="0" t="n">
-        <v>152.445413919916</v>
+        <v>152.1933647157504</v>
       </c>
       <c r="N29" s="0" t="n">
-        <v>-0.018013539323270482</v>
+        <v>-0.013066548205358191</v>
       </c>
       <c r="O29" s="0" t="n">
-        <v>-4028.228373377855</v>
+        <v>-4027.377333535692</v>
       </c>
       <c r="P29" s="0" t="n">
-        <v>-0.018013539323270482</v>
+        <v>-0.039034209645765074</v>
       </c>
       <c r="Q29" s="0" t="n">
-        <v>0.010356186377692743</v>
+        <v>0.011344982861500376</v>
       </c>
       <c r="R29" s="0" t="n">
-        <v>1678.8268336692147</v>
+        <v>1711.9574229552484</v>
       </c>
       <c r="S29" s="0" t="n">
-        <v>252.23881501921937</v>
+        <v>269.129787066478</v>
       </c>
       <c r="T29" s="0" t="n">
-        <v>529.6468865270227</v>
+        <v>530.2034897237013</v>
       </c>
       <c r="U29" s="0" t="n">
-        <v>373.9966713075509</v>
+        <v>361.9686819695657</v>
       </c>
     </row>
     <row r="30">
@@ -2028,64 +2028,64 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>2.800000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>938.8</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>168729.03766470906</v>
+        <v>168782.66854599296</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>466.35198973598455</v>
+        <v>466.2829581126147</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>1.3975547196494007</v>
+        <v>1.397925567241635</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.7900059793959933</v>
+        <v>0.7900043032712694</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>20388.260966030884</v>
+        <v>20310.596037332947</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00011372208726535539</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>0.010324746820579888</v>
+        <v>0.01113488559523612</v>
       </c>
       <c r="K30" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>0.0</v>
+        <v>41.879421577711305</v>
       </c>
       <c r="M30" s="0" t="n">
-        <v>152.545204810013</v>
+        <v>152.3096854296132</v>
       </c>
       <c r="N30" s="0" t="n">
-        <v>-0.017445698934170036</v>
+        <v>-0.014277422550236224</v>
       </c>
       <c r="O30" s="0" t="n">
-        <v>-4281.534802866486</v>
+        <v>-4274.019846371238</v>
       </c>
       <c r="P30" s="0" t="n">
-        <v>-0.017445698934170036</v>
+        <v>-0.06960531210103532</v>
       </c>
       <c r="Q30" s="0" t="n">
-        <v>0.010324746820579888</v>
+        <v>0.011248607682501476</v>
       </c>
       <c r="R30" s="0" t="n">
-        <v>1704.0507151711367</v>
+        <v>1739.295555941725</v>
       </c>
       <c r="S30" s="0" t="n">
-        <v>260.0659809821354</v>
+        <v>277.706732518368</v>
       </c>
       <c r="T30" s="0" t="n">
-        <v>567.0465536577778</v>
+        <v>567.0233090175029</v>
       </c>
       <c r="U30" s="0" t="n">
-        <v>387.1044611813605</v>
+        <v>374.5647710880216</v>
       </c>
     </row>
     <row r="31">
@@ -2093,64 +2093,64 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>2.9000000000000012</v>
+        <v>2.9</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>930.8999999999999</v>
+        <v>930.9</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>168768.62932609092</v>
+        <v>168825.43088539958</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>481.60651021698584</v>
+        <v>481.52921115461703</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>1.443709403509771</v>
+        <v>1.444111883325126</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>0.7798019537508547</v>
+        <v>0.7797080419280984</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>21407.39287930199</v>
+        <v>21318.089757584283</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>0.0</v>
+        <v>4.58606814092552e-06</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>0.010294298331908596</v>
+        <v>0.011108301184517546</v>
       </c>
       <c r="K31" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>0.0</v>
+        <v>1.7960541126964666</v>
       </c>
       <c r="M31" s="0" t="n">
-        <v>152.8481472095181</v>
+        <v>152.63133748705027</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>-0.016912755073937125</v>
+        <v>-0.016266084950173277</v>
       </c>
       <c r="O31" s="0" t="n">
-        <v>-4495.552504653418</v>
+        <v>-4477.176020456365</v>
       </c>
       <c r="P31" s="0" t="n">
-        <v>-0.016912755073937125</v>
+        <v>-0.08232338899647786</v>
       </c>
       <c r="Q31" s="0" t="n">
-        <v>0.010294298331908596</v>
+        <v>0.011112887252658472</v>
       </c>
       <c r="R31" s="0" t="n">
-        <v>1730.0573132693503</v>
+        <v>1767.4873099257602</v>
       </c>
       <c r="S31" s="0" t="n">
-        <v>267.874991717079</v>
+        <v>286.1975134098619</v>
       </c>
       <c r="T31" s="0" t="n">
-        <v>605.7569997759139</v>
+        <v>605.1067122306184</v>
       </c>
       <c r="U31" s="0" t="n">
-        <v>400.2347055116017</v>
+        <v>387.2484532095637</v>
       </c>
     </row>
     <row r="32">
@@ -2158,64 +2158,64 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>3.0000000000000013</v>
+        <v>3.0</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>922.9999999999999</v>
+        <v>923.0</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>168809.30212885435</v>
+        <v>168869.34762041166</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>496.89132493793767</v>
+        <v>496.80896870077567</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>1.489996884978846</v>
+        <v>1.4904442338195083</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>0.769001556837231</v>
+        <v>0.7688971755901928</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>22412.116680425923</v>
+        <v>22312.977409358937</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00010289862225064296</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>0.010264780005746238</v>
+        <v>0.011078201666837133</v>
       </c>
       <c r="K32" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>0.0</v>
+        <v>-42.77218741277289</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>153.17239605783232</v>
+        <v>152.96775313766656</v>
       </c>
       <c r="N32" s="0" t="n">
-        <v>-0.01641089779549305</v>
+        <v>-0.01815008858985746</v>
       </c>
       <c r="O32" s="0" t="n">
-        <v>-4706.544502889444</v>
+        <v>-4676.743096608694</v>
       </c>
       <c r="P32" s="0" t="n">
-        <v>-0.01641089779549305</v>
+        <v>-0.07120359294869741</v>
       </c>
       <c r="Q32" s="0" t="n">
-        <v>0.010264780005746238</v>
+        <v>0.010975303044586491</v>
       </c>
       <c r="R32" s="0" t="n">
-        <v>1756.8448124410581</v>
+        <v>1796.5232867686843</v>
       </c>
       <c r="S32" s="0" t="n">
-        <v>275.67779345923736</v>
+        <v>294.5895876107282</v>
       </c>
       <c r="T32" s="0" t="n">
-        <v>645.780470327074</v>
+        <v>644.4640578251776</v>
       </c>
       <c r="U32" s="0" t="n">
-        <v>413.40384975472256</v>
+        <v>400.04515526733906</v>
       </c>
     </row>
     <row r="33">
@@ -2223,64 +2223,64 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>3.1000000000000014</v>
+        <v>3.1</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>915.0999999999999</v>
+        <v>915.1</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>168851.04581319683</v>
+        <v>168914.3936540965</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>512.2085645437209</v>
+        <v>512.1226924564942</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>1.5364249680995372</v>
+        <v>1.5369253923450406</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>0.7581683529184308</v>
+        <v>0.7580515874279548</v>
       </c>
       <c r="H33" s="0" t="n">
-        <v>23415.07840241317</v>
+        <v>23305.55707142198</v>
       </c>
       <c r="I33" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00016918276399896905</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>0.010236137585772274</v>
+        <v>0.011045529646936317</v>
       </c>
       <c r="K33" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>0.0</v>
+        <v>-74.50398178386932</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>153.50470732567044</v>
+        <v>153.31241687012653</v>
       </c>
       <c r="N33" s="0" t="n">
-        <v>-0.01593740405207605</v>
+        <v>-0.019084477827985055</v>
       </c>
       <c r="O33" s="0" t="n">
-        <v>-4917.166464506766</v>
+        <v>-4878.521148824005</v>
       </c>
       <c r="P33" s="0" t="n">
-        <v>-0.01593740405207605</v>
+        <v>-0.03910107407230205</v>
       </c>
       <c r="Q33" s="0" t="n">
-        <v>0.010236137585772274</v>
+        <v>0.010876346882937347</v>
       </c>
       <c r="R33" s="0" t="n">
-        <v>1784.412591786982</v>
+        <v>1826.3940361927966</v>
       </c>
       <c r="S33" s="0" t="n">
-        <v>283.47614598886037</v>
+        <v>302.89757988252273</v>
       </c>
       <c r="T33" s="0" t="n">
-        <v>687.1208553025463</v>
+        <v>685.106325354488</v>
       </c>
       <c r="U33" s="0" t="n">
-        <v>426.61327715771034</v>
+        <v>412.94395289215663</v>
       </c>
     </row>
     <row r="34">
@@ -2288,64 +2288,64 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>3.2000000000000015</v>
+        <v>3.2</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>907.1999999999998</v>
+        <v>907.2</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>168893.85015754556</v>
+        <v>168960.54853658122</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>527.5590352762879</v>
+        <v>527.4716926061186</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>1.5829975045797253</v>
+        <v>1.5835607328622645</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>0.747301443263899</v>
+        <v>0.7471700235190493</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>24414.231841518536</v>
+        <v>24293.81905246439</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.0001686383882855736</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>0.010208321568279333</v>
+        <v>0.011012437098390447</v>
       </c>
       <c r="K34" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>0.0</v>
+        <v>-78.5408210037788</v>
       </c>
       <c r="M34" s="0" t="n">
-        <v>153.8475679543972</v>
+        <v>153.67458511257848</v>
       </c>
       <c r="N34" s="0" t="n">
-        <v>-0.015489899811175972</v>
+        <v>-0.018579042272734683</v>
       </c>
       <c r="O34" s="0" t="n">
-        <v>-5126.9886867188925</v>
+        <v>-5085.208428606728</v>
       </c>
       <c r="P34" s="0" t="n">
-        <v>-0.015489899811175972</v>
+        <v>0.0024962674426146463</v>
       </c>
       <c r="Q34" s="0" t="n">
-        <v>0.010208321568279333</v>
+        <v>0.010843798710104872</v>
       </c>
       <c r="R34" s="0" t="n">
-        <v>1812.760206385868</v>
+        <v>1857.0932687094482</v>
       </c>
       <c r="S34" s="0" t="n">
-        <v>291.27103597353704</v>
+        <v>311.16882955384096</v>
       </c>
       <c r="T34" s="0" t="n">
-        <v>729.7821830183173</v>
+        <v>727.0422096348183</v>
       </c>
       <c r="U34" s="0" t="n">
-        <v>439.86329615523744</v>
+        <v>425.91119498653285</v>
       </c>
     </row>
     <row r="35">
@@ -2353,64 +2353,64 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>3.3000000000000016</v>
+        <v>3.3</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>899.3</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>168937.7048619744</v>
+        <v>169007.8002553819</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>542.9437920717276</v>
+        <v>542.8578801439985</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>1.6297191086792917</v>
+        <v>1.6303575490298272</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>0.7363997512145348</v>
+        <v>0.7362507820122234</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>25407.539657327638</v>
+        <v>25275.774124899122</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00010114133659018309</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>0.010181286593028424</v>
+        <v>0.010981463599291374</v>
       </c>
       <c r="K35" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L35" s="0" t="n">
-        <v>0.0</v>
+        <v>-49.735905161986686</v>
       </c>
       <c r="M35" s="0" t="n">
-        <v>154.20353976374327</v>
+        <v>154.05570488626233</v>
       </c>
       <c r="N35" s="0" t="n">
-        <v>-0.015066262796850114</v>
+        <v>-0.01670486100428853</v>
       </c>
       <c r="O35" s="0" t="n">
-        <v>-5335.583328038803</v>
+        <v>-5297.4680261447975</v>
       </c>
       <c r="P35" s="0" t="n">
-        <v>-0.015066262796850114</v>
+        <v>0.037141083448482194</v>
       </c>
       <c r="Q35" s="0" t="n">
-        <v>0.010181286593028424</v>
+        <v>0.010880322262701192</v>
       </c>
       <c r="R35" s="0" t="n">
-        <v>1841.8873099832217</v>
+        <v>1888.6204291470472</v>
       </c>
       <c r="S35" s="0" t="n">
-        <v>299.063553574034</v>
+        <v>319.4671336609579</v>
       </c>
       <c r="T35" s="0" t="n">
-        <v>773.768512633841</v>
+        <v>770.2763806319672</v>
       </c>
       <c r="U35" s="0" t="n">
-        <v>453.1544463788237</v>
+        <v>438.9025273849394</v>
       </c>
     </row>
     <row r="36">
@@ -2418,64 +2418,64 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>3.4000000000000017</v>
+        <v>3.4</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>891.3999999999999</v>
+        <v>891.4000000000001</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>168982.5995648856</v>
+        <v>169056.14575077634</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>558.3641460481019</v>
+        <v>558.2828664843967</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>1.6765951819388816</v>
+        <v>1.6773223777711723</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>0.7254620164126551</v>
+        <v>0.7252923376275191</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>26392.973776526647</v>
+        <v>26249.385996583456</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>0.0</v>
+        <v>5.606500089005239e-06</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>0.010154991003850849</v>
+        <v>0.010954522126852504</v>
       </c>
       <c r="K36" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L36" s="0" t="n">
-        <v>0.0</v>
+        <v>2.9064344615417936</v>
       </c>
       <c r="M36" s="0" t="n">
-        <v>154.57526260384324</v>
+        <v>154.44961256035495</v>
       </c>
       <c r="N36" s="0" t="n">
-        <v>-0.014664589784769248</v>
+        <v>-0.014094347807270684</v>
       </c>
       <c r="O36" s="0" t="n">
-        <v>-5542.524493070596</v>
+        <v>-5512.981410519449</v>
       </c>
       <c r="P36" s="0" t="n">
-        <v>-0.014664589784769248</v>
+        <v>0.04990154594926526</v>
       </c>
       <c r="Q36" s="0" t="n">
-        <v>0.010154991003850849</v>
+        <v>0.01096012862694151</v>
       </c>
       <c r="R36" s="0" t="n">
-        <v>1871.793665340625</v>
+        <v>1920.9811284678055</v>
       </c>
       <c r="S36" s="0" t="n">
-        <v>306.85489796652007</v>
+        <v>327.8474574424243</v>
       </c>
       <c r="T36" s="0" t="n">
-        <v>819.0839572717234</v>
+        <v>814.8092512463468</v>
       </c>
       <c r="U36" s="0" t="n">
-        <v>466.4875037833089</v>
+        <v>451.88029793140186</v>
       </c>
     </row>
     <row r="37">
@@ -2483,64 +2483,64 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>3.5000000000000018</v>
+        <v>3.5</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>883.4999999999999</v>
+        <v>883.5</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>169028.523860134</v>
+        <v>169105.5875996573</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>573.8216723084862</v>
+        <v>573.7477591530951</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>1.723631939066168</v>
+        <v>1.724460358569628</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0.7144867887618739</v>
+        <v>0.714293491153873</v>
       </c>
       <c r="H37" s="0" t="n">
-        <v>27368.51533551225</v>
+        <v>27212.560093075088</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>0.0</v>
+        <v>0.000105695234766083</v>
       </c>
       <c r="J37" s="0" t="n">
-        <v>0.010129396466330993</v>
+        <v>0.010932091230667186</v>
       </c>
       <c r="K37" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L37" s="0" t="n">
-        <v>0.0</v>
+        <v>57.678074968204044</v>
       </c>
       <c r="M37" s="0" t="n">
-        <v>154.9654581644859</v>
+        <v>154.85466057284168</v>
       </c>
       <c r="N37" s="0" t="n">
-        <v>-0.014283168868146961</v>
+        <v>-0.01170500999295658</v>
       </c>
       <c r="O37" s="0" t="n">
-        <v>-5747.388220457572</v>
+        <v>-5726.750015289092</v>
       </c>
       <c r="P37" s="0" t="n">
-        <v>-0.014283168868146961</v>
+        <v>0.03431815932994765</v>
       </c>
       <c r="Q37" s="0" t="n">
-        <v>0.010129396466330993</v>
+        <v>0.011037786465433271</v>
       </c>
       <c r="R37" s="0" t="n">
-        <v>1902.479155137277</v>
+        <v>1954.1850133200248</v>
       </c>
       <c r="S37" s="0" t="n">
-        <v>314.64638280231685</v>
+        <v>336.33198046096436</v>
       </c>
       <c r="T37" s="0" t="n">
-        <v>865.7327076500543</v>
+        <v>860.6385156844236</v>
       </c>
       <c r="U37" s="0" t="n">
-        <v>479.86348621282445</v>
+        <v>464.83038847777965</v>
       </c>
     </row>
     <row r="38">
@@ -2548,64 +2548,64 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>3.600000000000002</v>
+        <v>3.6</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>875.5999999999999</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>169075.46731454483</v>
+        <v>169156.1280169078</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>589.3182181249348</v>
+        <v>589.2540714054436</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>1.7708364351880712</v>
+        <v>1.7717778948625391</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>0.7034724220682618</v>
+        <v>0.7032527484580392</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>28332.15414677401</v>
+        <v>28163.215943997315</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00015427988533407838</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>0.010104467633894242</v>
+        <v>0.010912981880110478</v>
       </c>
       <c r="K38" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L38" s="0" t="n">
-        <v>0.0</v>
+        <v>88.49989501733789</v>
       </c>
       <c r="M38" s="0" t="n">
-        <v>155.3769345054266</v>
+        <v>155.28040749297637</v>
       </c>
       <c r="N38" s="0" t="n">
-        <v>-0.013920455833398999</v>
+        <v>-0.010415816972501771</v>
       </c>
       <c r="O38" s="0" t="n">
-        <v>-5949.752370822542</v>
+        <v>-5932.8603261930775</v>
       </c>
       <c r="P38" s="0" t="n">
-        <v>-0.013920455833398999</v>
+        <v>-0.0034259245129865026</v>
       </c>
       <c r="Q38" s="0" t="n">
-        <v>0.010104467633894242</v>
+        <v>0.011067261765444557</v>
       </c>
       <c r="R38" s="0" t="n">
-        <v>1933.9437934175087</v>
+        <v>1988.2417879889235</v>
       </c>
       <c r="S38" s="0" t="n">
-        <v>322.4394416683525</v>
+        <v>344.8989114167717</v>
       </c>
       <c r="T38" s="0" t="n">
-        <v>913.7190562713367</v>
+        <v>907.7620348129776</v>
       </c>
       <c r="U38" s="0" t="n">
-        <v>493.28365944003184</v>
+        <v>477.77097188026977</v>
       </c>
     </row>
     <row r="39">
@@ -2613,64 +2613,64 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>3.700000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>867.6999999999998</v>
+        <v>867.7</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>169123.41948578475</v>
+        <v>169207.76271658702</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>604.8559115754774</v>
+        <v>604.8044642604694</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>1.8182165946977968</v>
+        <v>1.8192848005467064</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>0.692417067309379</v>
+        <v>0.6921678196340354</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>29281.88767319999</v>
+        <v>29099.348396891797</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>0.0</v>
+        <v>0.0001288093647322436</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>0.010080171855127114</v>
+        <v>0.010894840032039594</v>
       </c>
       <c r="K39" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L39" s="0" t="n">
-        <v>0.0</v>
+        <v>77.56788313762904</v>
       </c>
       <c r="M39" s="0" t="n">
-        <v>155.81259137627436</v>
+        <v>155.737662063012</v>
       </c>
       <c r="N39" s="0" t="n">
-        <v>-0.013575053950813015</v>
+        <v>-0.010620975814305612</v>
       </c>
       <c r="O39" s="0" t="n">
-        <v>-6149.196411371998</v>
+        <v>-6127.152418806179</v>
       </c>
       <c r="P39" s="0" t="n">
-        <v>-0.013575053950813015</v>
+        <v>-0.04598629246401331</v>
       </c>
       <c r="Q39" s="0" t="n">
-        <v>0.010080171855127114</v>
+        <v>0.011023649396771838</v>
       </c>
       <c r="R39" s="0" t="n">
-        <v>1966.187737584344</v>
+        <v>2023.1570618274184</v>
       </c>
       <c r="S39" s="0" t="n">
-        <v>330.2356336102926</v>
+        <v>353.4908641647371</v>
       </c>
       <c r="T39" s="0" t="n">
-        <v>963.0474222153399</v>
+        <v>956.1809255902377</v>
       </c>
       <c r="U39" s="0" t="n">
-        <v>506.74954372136375</v>
+        <v>490.74703151568923</v>
       </c>
     </row>
     <row r="40">
@@ -2678,64 +2678,64 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>3.800000000000002</v>
+        <v>3.8</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>859.7999999999998</v>
+        <v>859.8</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>169172.3699405543</v>
+        <v>169260.47751131366</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>620.4371707131048</v>
+        <v>620.4021985387304</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>1.8657812419476256</v>
+        <v>1.8669925949521227</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>0.6813186654726346</v>
+        <v>0.6810360168420364</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>30215.719493209035</v>
+        <v>30018.99623946398</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>0.0</v>
+        <v>4.1633061305380754e-05</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>0.01005647891636936</v>
+        <v>0.010875214176941733</v>
       </c>
       <c r="K40" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L40" s="0" t="n">
-        <v>0.0</v>
+        <v>26.286155527873678</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>156.2754264002354</v>
+        <v>156.22675207684458</v>
       </c>
       <c r="N40" s="0" t="n">
-        <v>-0.013245696616588382</v>
+        <v>-0.012021843758394341</v>
       </c>
       <c r="O40" s="0" t="n">
-        <v>-6345.301093573898</v>
+        <v>-6309.509302948289</v>
       </c>
       <c r="P40" s="0" t="n">
-        <v>-0.013245696616588382</v>
+        <v>-0.072452356245272</v>
       </c>
       <c r="Q40" s="0" t="n">
-        <v>0.01005647891636936</v>
+        <v>0.010916847238247115</v>
       </c>
       <c r="R40" s="0" t="n">
-        <v>1999.2113009453733</v>
+        <v>2058.9299680937343</v>
       </c>
       <c r="S40" s="0" t="n">
-        <v>338.0366487800939</v>
+        <v>362.0409971689158</v>
       </c>
       <c r="T40" s="0" t="n">
-        <v>1013.7223765874763</v>
+        <v>1005.9013622066072</v>
       </c>
       <c r="U40" s="0" t="n">
-        <v>520.2629209198036</v>
+        <v>503.81068301558213</v>
       </c>
     </row>
     <row r="41">
@@ -2743,64 +2743,64 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>3.900000000000002</v>
+        <v>3.9</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>851.8999999999999</v>
+        <v>851.9000000000001</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>169222.30827307707</v>
+        <v>169314.2495169451</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>636.0647133531284</v>
+        <v>636.0502163261386</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>1.9135401340623435</v>
+        <v>1.9149117397322082</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>0.6701749398988313</v>
+        <v>0.6698548990330647</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>31131.65723784999</v>
+        <v>30920.17925117564</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>0.0</v>
+        <v>-6.39933944497339e-05</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>0.010033360814601386</v>
+        <v>0.010852710879550425</v>
       </c>
       <c r="K41" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L41" s="0" t="n">
-        <v>0.0</v>
+        <v>-42.3115615273782</v>
       </c>
       <c r="M41" s="0" t="n">
-        <v>156.76854220298011</v>
+        <v>156.7433689910693</v>
       </c>
       <c r="N41" s="0" t="n">
-        <v>-0.01293123238648449</v>
+        <v>-0.013747664478625535</v>
       </c>
       <c r="O41" s="0" t="n">
-        <v>-6537.648019948498</v>
+        <v>-6484.352214826135</v>
       </c>
       <c r="P41" s="0" t="n">
-        <v>-0.01293123238648449</v>
+        <v>-0.06889617646950426</v>
       </c>
       <c r="Q41" s="0" t="n">
-        <v>0.010033360814601386</v>
+        <v>0.010788717485100692</v>
       </c>
       <c r="R41" s="0" t="n">
-        <v>2033.0149658233827</v>
+        <v>2095.553867436569</v>
       </c>
       <c r="S41" s="0" t="n">
-        <v>345.8443142703734</v>
+        <v>370.50625379782593</v>
       </c>
       <c r="T41" s="0" t="n">
-        <v>1065.7486686794566</v>
+        <v>1056.9340388270982</v>
       </c>
       <c r="U41" s="0" t="n">
-        <v>533.8258422555549</v>
+        <v>516.9961253096862</v>
       </c>
     </row>
     <row r="42">
@@ -2808,64 +2808,64 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>4.000000000000002</v>
+        <v>4.0</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>843.9999999999999</v>
+        <v>844.0</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>169273.22412386976</v>
+        <v>169369.05275951658</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>651.7415675734263</v>
+        <v>651.7514066471947</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>1.9615039961745595</v>
+        <v>1.9630525078891086</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>0.6589833880606015</v>
+        <v>0.6586220691767106</v>
       </c>
       <c r="H42" s="0" t="n">
-        <v>32027.709978675008</v>
+        <v>31800.90483659562</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00013440538929987257</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>0.010010791556452918</v>
+        <v>0.010827663911714322</v>
       </c>
       <c r="K42" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L42" s="0" t="n">
-        <v>0.0</v>
+        <v>-92.95709056621345</v>
       </c>
       <c r="M42" s="0" t="n">
-        <v>157.29515457626843</v>
+        <v>157.2922731410193</v>
       </c>
       <c r="N42" s="0" t="n">
-        <v>-0.012630612024126199</v>
+        <v>-0.014774642846382859</v>
       </c>
       <c r="O42" s="0" t="n">
-        <v>-6725.8190955217515</v>
+        <v>-6658.669026666175</v>
       </c>
       <c r="P42" s="0" t="n">
-        <v>-0.012630612024126199</v>
+        <v>-0.036294107400301555</v>
       </c>
       <c r="Q42" s="0" t="n">
-        <v>0.010010791556452918</v>
+        <v>0.010693258522414449</v>
       </c>
       <c r="R42" s="0" t="n">
-        <v>2067.59939725042</v>
+        <v>2133.0200752134965</v>
       </c>
       <c r="S42" s="0" t="n">
-        <v>353.6606001994707</v>
+        <v>378.89173070765986</v>
       </c>
       <c r="T42" s="0" t="n">
-        <v>1119.1312529050122</v>
+        <v>1109.2914196225713</v>
       </c>
       <c r="U42" s="0" t="n">
-        <v>547.4406367539929</v>
+        <v>530.3026989069083</v>
       </c>
     </row>
     <row r="43">
@@ -2873,64 +2873,64 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>4.100000000000001</v>
+        <v>4.1</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>836.0999999999999</v>
+        <v>836.1</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>169325.1071987825</v>
+        <v>169424.8656730916</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>667.4710830310531</v>
+        <v>667.5093814380394</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>2.0096845594122525</v>
+        <v>2.011427438367258</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>0.647960543931521</v>
+        <v>0.6475949957032492</v>
       </c>
       <c r="H43" s="0" t="n">
-        <v>32913.022879511336</v>
+        <v>32672.334982704815</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00013310182922812142</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>0.009988746979816618</v>
+        <v>0.010801947522856918</v>
       </c>
       <c r="K43" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L43" s="0" t="n">
-        <v>0.0</v>
+        <v>-96.18854473610473</v>
       </c>
       <c r="M43" s="0" t="n">
-        <v>157.8452805974579</v>
+        <v>157.86873631486782</v>
       </c>
       <c r="N43" s="0" t="n">
-        <v>-0.012342877253401337</v>
+        <v>-0.014445595912723739</v>
       </c>
       <c r="O43" s="0" t="n">
-        <v>-6911.73480469738</v>
+        <v>-6840.990751973429</v>
       </c>
       <c r="P43" s="0" t="n">
-        <v>-0.012342877253401337</v>
+        <v>0.008920124753153985</v>
       </c>
       <c r="Q43" s="0" t="n">
-        <v>0.009988746979816618</v>
+        <v>0.010668845693628796</v>
       </c>
       <c r="R43" s="0" t="n">
-        <v>2102.965457270367</v>
+        <v>2171.3229693701614</v>
       </c>
       <c r="S43" s="0" t="n">
-        <v>361.4876261133867</v>
+        <v>387.25185154889095</v>
       </c>
       <c r="T43" s="0" t="n">
-        <v>1173.8753165804114</v>
+        <v>1162.9841249812225</v>
       </c>
       <c r="U43" s="0" t="n">
-        <v>561.1099204697377</v>
+        <v>543.695482581702</v>
       </c>
     </row>
     <row r="44">
@@ -2938,64 +2938,64 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>4.200000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>828.1999999999999</v>
+        <v>828.2</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>169377.94728831027</v>
+        <v>169481.67645798827</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>683.2556110907989</v>
+        <v>683.3235120627098</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>2.0580905894192547</v>
+        <v>2.06003647924165</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>0.6379760165464731</v>
+        <v>0.6375819354154966</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>33833.21318030158</v>
+        <v>33576.47710595645</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>0.0</v>
+        <v>-6.1026978410598364e-05</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>0.00996720459509248</v>
+        <v>0.010777990466441149</v>
       </c>
       <c r="K44" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>0.0</v>
+        <v>-46.03452139293188</v>
       </c>
       <c r="M44" s="0" t="n">
-        <v>158.36451763821148</v>
+        <v>158.42146937673553</v>
       </c>
       <c r="N44" s="0" t="n">
-        <v>-0.01206717448476066</v>
+        <v>-0.012821179410413639</v>
       </c>
       <c r="O44" s="0" t="n">
-        <v>-7104.974767863331</v>
+        <v>-7041.392942758339</v>
       </c>
       <c r="P44" s="0" t="n">
-        <v>-0.01206717448476066</v>
+        <v>0.04271380861838805</v>
       </c>
       <c r="Q44" s="0" t="n">
-        <v>0.00996720459509248</v>
+        <v>0.010716963488030551</v>
       </c>
       <c r="R44" s="0" t="n">
-        <v>2139.1142198817056</v>
+        <v>2210.463740789682</v>
       </c>
       <c r="S44" s="0" t="n">
-        <v>369.3269477110043</v>
+        <v>395.66198025834547</v>
       </c>
       <c r="T44" s="0" t="n">
-        <v>1229.9863086273851</v>
+        <v>1218.018139794959</v>
       </c>
       <c r="U44" s="0" t="n">
-        <v>574.8354858405439</v>
+        <v>557.1199327934345</v>
       </c>
     </row>
     <row r="45">
@@ -3003,64 +3003,64 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>4.300000000000001</v>
+        <v>4.3</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>820.3</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>169431.7341825086</v>
+        <v>169539.48316342197</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>699.09206285462</v>
+        <v>699.1933563210894</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>2.106714494429266</v>
+        <v>2.108880336458486</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>0.6282975897956673</v>
+        <v>0.6278746708763803</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>34752.74470266045</v>
+        <v>34479.39927292644</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>0.0</v>
+        <v>4.211579740211031e-05</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>0.00994614340247531</v>
+        <v>0.010757475628681018</v>
       </c>
       <c r="K45" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>0.0</v>
+        <v>33.12793733740825</v>
       </c>
       <c r="M45" s="0" t="n">
-        <v>158.89529769374738</v>
+        <v>158.98169059137297</v>
       </c>
       <c r="N45" s="0" t="n">
-        <v>-0.011802816298463359</v>
+        <v>-0.010665637244926009</v>
       </c>
       <c r="O45" s="0" t="n">
-        <v>-7298.0763875586945</v>
+        <v>-7247.63071415541</v>
       </c>
       <c r="P45" s="0" t="n">
-        <v>-0.011802816298463359</v>
+        <v>0.046100588111951266</v>
       </c>
       <c r="Q45" s="0" t="n">
-        <v>0.00994614340247531</v>
+        <v>0.010799591426083128</v>
       </c>
       <c r="R45" s="0" t="n">
-        <v>2176.046914652806</v>
+        <v>2250.4505817272784</v>
       </c>
       <c r="S45" s="0" t="n">
-        <v>377.17716574431927</v>
+        <v>404.1806960354159</v>
       </c>
       <c r="T45" s="0" t="n">
-        <v>1287.4698572114396</v>
+        <v>1274.3943115889617</v>
       </c>
       <c r="U45" s="0" t="n">
-        <v>588.6145580831401</v>
+        <v>570.5342360243393</v>
       </c>
     </row>
     <row r="46">
@@ -3074,58 +3074,58 @@
         <v>812.4</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>169486.45724129162</v>
+        <v>169598.28856941604</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>714.9815926239947</v>
+        <v>715.1194784687932</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>2.155561476721884</v>
+        <v>2.1579628834821483</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>0.618929014266409</v>
+        <v>0.6184775948939485</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>35672.390084821294</v>
+        <v>35381.78519717623</v>
       </c>
       <c r="I46" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00011808484055996318</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>0.009925543601933685</v>
+        <v>0.010740408463922432</v>
       </c>
       <c r="K46" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L46" s="0" t="n">
-        <v>0.0</v>
+        <v>96.76372059901489</v>
       </c>
       <c r="M46" s="0" t="n">
-        <v>159.43700854971803</v>
+        <v>159.5481027004898</v>
       </c>
       <c r="N46" s="0" t="n">
-        <v>-0.011549097323503999</v>
+        <v>-0.009047940414469489</v>
       </c>
       <c r="O46" s="0" t="n">
-        <v>-7491.201917812472</v>
+        <v>-7450.4952727328</v>
       </c>
       <c r="P46" s="0" t="n">
-        <v>-0.011549097323503999</v>
+        <v>0.01646239584001155</v>
       </c>
       <c r="Q46" s="0" t="n">
-        <v>0.009925543601933685</v>
+        <v>0.010858493304482393</v>
       </c>
       <c r="R46" s="0" t="n">
-        <v>2213.764631227238</v>
+        <v>2291.2952666369297</v>
       </c>
       <c r="S46" s="0" t="n">
-        <v>385.03916351625753</v>
+        <v>412.8162461176857</v>
       </c>
       <c r="T46" s="0" t="n">
-        <v>1346.3313130197537</v>
+        <v>1332.1110372985195</v>
       </c>
       <c r="U46" s="0" t="n">
-        <v>602.4479399498721</v>
+        <v>583.9337423259433</v>
       </c>
     </row>
     <row r="47">
@@ -3139,58 +3139,58 @@
         <v>804.5</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>169542.10573005924</v>
+        <v>169658.09190451543</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>730.9252934789665</v>
+        <v>731.1029083435964</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>2.2046365837302777</v>
+        <v>2.207289397464616</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>0.6098742416854153</v>
+        <v>0.6093949852916336</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>36593.05084631727</v>
+        <v>36284.4881005326</v>
       </c>
       <c r="I47" s="0" t="n">
-        <v>0.0</v>
+        <v>0.00012294968293992915</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>0.009905386624540843</v>
+        <v>0.01072509689700577</v>
       </c>
       <c r="K47" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L47" s="0" t="n">
-        <v>0.0</v>
+        <v>104.86056141773541</v>
       </c>
       <c r="M47" s="0" t="n">
-        <v>159.9888527386172</v>
+        <v>160.1293354427684</v>
       </c>
       <c r="N47" s="0" t="n">
-        <v>-0.011305370780392803</v>
+        <v>-0.008741350078832245</v>
       </c>
       <c r="O47" s="0" t="n">
-        <v>-7684.540677726625</v>
+        <v>-7641.763219009571</v>
       </c>
       <c r="P47" s="0" t="n">
-        <v>-0.011305370780392803</v>
+        <v>-0.029401340148170706</v>
       </c>
       <c r="Q47" s="0" t="n">
-        <v>0.009905386624540843</v>
+        <v>0.0108480465799457</v>
       </c>
       <c r="R47" s="0" t="n">
-        <v>2252.268547578864</v>
+        <v>2333.0074419810903</v>
       </c>
       <c r="S47" s="0" t="n">
-        <v>392.9137768548929</v>
+        <v>421.5190930711661</v>
       </c>
       <c r="T47" s="0" t="n">
-        <v>1406.576107014741</v>
+        <v>1391.1683513132957</v>
       </c>
       <c r="U47" s="0" t="n">
-        <v>616.3363924067253</v>
+        <v>597.3551010621126</v>
       </c>
     </row>
     <row r="48">
@@ -3204,58 +3204,58 @@
         <v>796.6</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>169598.66881299633</v>
+        <v>169718.8822339665</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>746.9241787528282</v>
+        <v>747.1453011714741</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>2.2539446525487303</v>
+        <v>2.256866914235066</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>0.6011374306139354</v>
+        <v>0.600630996628132</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>37515.75879534279</v>
+        <v>37188.56489465571</v>
       </c>
       <c r="I48" s="0" t="n">
-        <v>0.0</v>
+        <v>5.412890486927128e-05</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>0.009885655030213183</v>
+        <v>0.010709115041486453</v>
       </c>
       <c r="K48" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L48" s="0" t="n">
-        <v>0.0</v>
+        <v>48.005783253372385</v>
       </c>
       <c r="M48" s="0" t="n">
-        <v>160.5498366501604</v>
+        <v>160.72645498368377</v>
       </c>
       <c r="N48" s="0" t="n">
-        <v>-0.011071042781014296</v>
+        <v>-0.009758194339028583</v>
       </c>
       <c r="O48" s="0" t="n">
-        <v>-7878.309347021985</v>
+        <v>-7819.679842360907</v>
       </c>
       <c r="P48" s="0" t="n">
-        <v>-0.011071042781014296</v>
+        <v>-0.06399004881861182</v>
       </c>
       <c r="Q48" s="0" t="n">
-        <v>0.009885655030213183</v>
+        <v>0.010763243946355725</v>
       </c>
       <c r="R48" s="0" t="n">
-        <v>2291.5599252643533</v>
+        <v>2375.5899440327216</v>
       </c>
       <c r="S48" s="0" t="n">
-        <v>400.8017852453733</v>
+        <v>430.20919534214664</v>
       </c>
       <c r="T48" s="0" t="n">
-        <v>1468.2097462554134</v>
+        <v>1451.5712927569155</v>
       </c>
       <c r="U48" s="0" t="n">
-        <v>630.2806182564307</v>
+        <v>610.8568975674053</v>
       </c>
     </row>
     <row r="49">
@@ -3263,64 +3263,64 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>4.699999999999999</v>
+        <v>4.7</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>788.7</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>169656.13554521886</v>
+        <v>169780.63758666575</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>762.9791624178442</v>
+        <v>763.2478163922717</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>2.3034902509396566</v>
+        <v>2.306700803817831</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>0.5927229502275613</v>
+        <v>0.5921902946728237</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>38441.677304224584</v>
+        <v>38095.21119883268</v>
       </c>
       <c r="I49" s="0" t="n">
-        <v>0.0</v>
+        <v>-4.614989121207299e-05</v>
       </c>
       <c r="J49" s="0" t="n">
-        <v>0.009866332415397397</v>
+        <v>0.010690732243068187</v>
       </c>
       <c r="K49" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L49" s="0" t="n">
-        <v>0.0</v>
+        <v>-42.52481400857432</v>
       </c>
       <c r="M49" s="0" t="n">
-        <v>161.11875914600682</v>
+        <v>161.33044257724214</v>
       </c>
       <c r="N49" s="0" t="n">
-        <v>-0.01084556729296586</v>
+        <v>-0.01132104178164187</v>
       </c>
       <c r="O49" s="0" t="n">
-        <v>-8072.752233887162</v>
+        <v>-7991.064140813061</v>
       </c>
       <c r="P49" s="0" t="n">
-        <v>-0.01084556729296586</v>
+        <v>-0.06563144964264817</v>
       </c>
       <c r="Q49" s="0" t="n">
-        <v>0.009866332415397397</v>
+        <v>0.010644582351856115</v>
       </c>
       <c r="R49" s="0" t="n">
-        <v>2331.6401037888904</v>
+        <v>2419.038036144288</v>
       </c>
       <c r="S49" s="0" t="n">
-        <v>408.7039023864201</v>
+        <v>438.8235876090381</v>
       </c>
       <c r="T49" s="0" t="n">
-        <v>1531.2378080810565</v>
+        <v>1513.3304150801534</v>
       </c>
       <c r="U49" s="0" t="n">
-        <v>644.2812448441649</v>
+        <v>624.4846580865728</v>
       </c>
     </row>
     <row r="50">
@@ -3334,58 +3334,58 @@
         <v>786.3299999999999</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>169731.95543565945</v>
+        <v>169799.3482767274</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>783.9246011068253</v>
+        <v>768.09036616557</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>2.368223378948551</v>
+        <v>2.321701444736232</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>0.5822795451462839</v>
+        <v>0.5897218982475056</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>39652.213541334706</v>
+        <v>38367.89831077787</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>0.0</v>
+        <v>-7.2891001756845e-05</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>0.009841724603791246</v>
+        <v>0.010684698747795455</v>
       </c>
       <c r="K50" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L50" s="0" t="n">
-        <v>0.0</v>
+        <v>-67.92932756606261</v>
       </c>
       <c r="M50" s="0" t="n">
-        <v>160.18889881333513</v>
+        <v>161.51235099095754</v>
       </c>
       <c r="N50" s="0" t="n">
-        <v>-0.010565041931274208</v>
+        <v>-0.011727490707897473</v>
       </c>
       <c r="O50" s="0" t="n">
-        <v>-8326.964843680287</v>
+        <v>-8042.99348647448</v>
       </c>
       <c r="P50" s="0" t="n">
-        <v>-0.010563303995961911</v>
+        <v>-0.058810743611964346</v>
       </c>
       <c r="Q50" s="0" t="n">
-        <v>0.009841724603791246</v>
+        <v>0.010611807746038609</v>
       </c>
       <c r="R50" s="0" t="n">
-        <v>2384.7716110991255</v>
+        <v>2432.239982274428</v>
       </c>
       <c r="S50" s="0" t="n">
-        <v>418.9899723708781</v>
+        <v>441.39049859952075</v>
       </c>
       <c r="T50" s="0" t="n">
-        <v>1614.9943699107992</v>
+        <v>1532.1245897339418</v>
       </c>
       <c r="U50" s="0" t="n">
-        <v>662.5595696034779</v>
+        <v>628.5994259800322</v>
       </c>
     </row>
     <row r="51">
@@ -3393,64 +3393,64 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>4.799999999999999</v>
+        <v>4.8</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>780.8000000000001</v>
+        <v>780.8</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>169714.49486373385</v>
+        <v>169843.3307035984</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>779.0910383324449</v>
+        <v>779.4109405805655</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>2.3532776146616934</v>
+        <v>2.3567943180472244</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>0.5846353819815842</v>
+        <v>0.5840780685517606</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>39372.10239244569</v>
+        <v>39005.738571696515</v>
       </c>
       <c r="I51" s="0" t="n">
-        <v>0.0</v>
+        <v>-0.00011545920512064183</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>0.00984740332954651</v>
+        <v>0.010669953285836344</v>
       </c>
       <c r="K51" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="L51" s="0" t="n">
-        <v>0.0</v>
+        <v>-110.44569965283213</v>
       </c>
       <c r="M51" s="0" t="n">
-        <v>161.69419972203178</v>
+        <v>161.93953466584549</v>
       </c>
       <c r="N51" s="0" t="n">
-        <v>-0.010628441679885902</v>
+        <v>-0.012322980407627354</v>
       </c>
       <c r="O51" s="0" t="n">
-        <v>-8268.141502413595</v>
+        <v>-8168.011503129173</v>
       </c>
       <c r="P51" s="0" t="n">
-        <v>-0.010628441679885902</v>
+        <v>-0.03263003511743359</v>
       </c>
       <c r="Q51" s="0" t="n">
-        <v>0.00984740332954651</v>
+        <v>0.0105544940807157</v>
       </c>
       <c r="R51" s="0" t="n">
-        <v>2372.5104940275323</v>
+        <v>2463.3433076114106</v>
       </c>
       <c r="S51" s="0" t="n">
-        <v>416.62076615285804</v>
+        <v>447.35691429071034</v>
       </c>
       <c r="T51" s="0" t="n">
-        <v>1595.665932565473</v>
+        <v>1576.458914292164</v>
       </c>
       <c r="U51" s="0" t="n">
-        <v>658.3388057984525</v>
+        <v>638.242278083312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>